<commit_message>
Adding unique unit IDs instead of just unit names
</commit_message>
<xml_diff>
--- a/data/demo/factories/cementFactory_withCCS.xlsx
+++ b/data/demo/factories/cementFactory_withCCS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1695" windowWidth="27645" windowHeight="16545" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="1455" yWindow="1695" windowWidth="27645" windowHeight="16545"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -689,7 +689,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated to include single-unit-only chain shortcut
</commit_message>
<xml_diff>
--- a/data/demo/factories/cementFactory_withCCS.xlsx
+++ b/data/demo/factories/cementFactory_withCCS.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\demo\factories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/demo/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5573CD3B-AE2C-8241-9313-A07671ED49E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1695" windowWidth="27645" windowHeight="16545"/>
+    <workbookView xWindow="1460" yWindow="1700" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
     <sheet name="Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Cement Chain" sheetId="3" r:id="rId3"/>
-    <sheet name="Power Chain" sheetId="4" r:id="rId4"/>
-    <sheet name="CO2 Capture" sheetId="5" r:id="rId5"/>
+    <sheet name="CO2 Capture" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="cementFactoryChains" localSheetId="0">'Chain List'!$A$1:$D$4</definedName>
+    <definedName name="cementFactoryChains" localSheetId="0">'Chain List'!$A$1:$C$4</definedName>
     <definedName name="cementFactoryConnections" localSheetId="1">Connections!$B$1:$F$4</definedName>
     <definedName name="cementFlow" localSheetId="2">'Cement Chain'!$A$1:$C$4</definedName>
-    <definedName name="CO2CapFlow" localSheetId="4">'CO2 Capture'!$A$1:$C$3</definedName>
-    <definedName name="powerFlow" localSheetId="3">'Power Chain'!$A$1:$C$2</definedName>
+    <definedName name="CO2CapFlow" localSheetId="3">'CO2 Capture'!$A$1:$C$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,8 +34,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="cementFactoryChains" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="cementFactoryChains" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/cementFactoryChains.tsv" thousands=" ">
       <textFields count="4">
         <textField/>
@@ -46,7 +45,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="cementFactoryConnections" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="cementFactoryConnections" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/cementFactoryConnections.tsv" thousands=" ">
       <textFields count="6">
         <textField/>
@@ -58,7 +57,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="cementFlow" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="cementFlow" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/cementFlow.tsv" thousands=" ">
       <textFields count="3">
         <textField/>
@@ -67,17 +66,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="CO2CapFlow" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="CO2CapFlow" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/CO2CapFlow.tsv" thousands=" ">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="5" name="powerFlow" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/chainFiles/powerFlow.tsv" thousands=" ">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -89,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>ChainName</t>
   </si>
@@ -100,9 +90,6 @@
     <t>Product_IO</t>
   </si>
   <si>
-    <t>ChainFile</t>
-  </si>
-  <si>
     <t>cement</t>
   </si>
   <si>
@@ -172,15 +159,6 @@
     <t>CO2 Capture</t>
   </si>
   <si>
-    <t>here</t>
-  </si>
-  <si>
-    <t>thisfile</t>
-  </si>
-  <si>
-    <t>same</t>
-  </si>
-  <si>
     <t>Recycle_Replacing</t>
   </si>
   <si>
@@ -225,11 +203,14 @@
   <si>
     <t>demo_powerstation</t>
   </si>
+  <si>
+    <t>This Unit Only</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -280,23 +261,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cementFactoryChains" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cementFactoryChains" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cementFactoryConnections" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cementFactoryConnections" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cementFlow" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cementFlow" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="powerFlow" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="CO2CapFlow" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="CO2CapFlow" connectionId="4" xr16:uid="{00000000-0016-0000-0400-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,23 +572,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,61 +598,55 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -685,18 +655,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
@@ -705,122 +675,122 @@
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I5">
         <v>0.2</v>
@@ -832,62 +802,62 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -896,93 +866,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>